<commit_message>
Am incercat cu sendgrid. Am inceput cu google api
</commit_message>
<xml_diff>
--- a/payslips.xlsx
+++ b/payslips.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">nume1</t>
   </si>
   <si>
-    <t xml:space="preserve">nume1@gmail.com</t>
+    <t xml:space="preserve">NumilenMercado@yandex.com</t>
   </si>
   <si>
     <t xml:space="preserve">dirnume1/payslip.pdf</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">nume2</t>
   </si>
   <si>
-    <t xml:space="preserve">nume2@gmail.com</t>
+    <t xml:space="preserve">lupascugabrielcristian@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">nume3</t>
@@ -88,6 +88,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,8 +148,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,107 +170,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Can attach pdf files
</commit_message>
<xml_diff>
--- a/payslips.xlsx
+++ b/payslips.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -37,19 +37,25 @@
     <t xml:space="preserve">NumilenMercado@yandex.com</t>
   </si>
   <si>
+    <t xml:space="preserve">pers1/payslip.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nume2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lupascugabrielcristian@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pers2/payslip.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nume3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nume3@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">dirnume1/payslip.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nume2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lupascugabrielcristian@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nume3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nume3@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">nume4</t>
@@ -170,20 +176,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,62 +222,62 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>